<commit_message>
Using js to optimize and make the process faster
</commit_message>
<xml_diff>
--- a/Files_and_Tags.xlsx
+++ b/Files_and_Tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh16.Yadav\Desktop\github\DamnIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AACBBD-37C8-46C0-8E63-1B8D309035B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8001E5-0EEE-4FBA-AFE3-EA66FBE86561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
   <si>
     <t>FileNames</t>
   </si>
@@ -160,7 +160,115 @@
     <t>000044.jpg</t>
   </si>
   <si>
-    <t>Australia, India, Indian Prime Minister, Australian Prime Minister, Anthony, Modi, Bilateral Relations, International Relations, Trade, Pact, Harmony</t>
+    <t>000045.jpg</t>
+  </si>
+  <si>
+    <t>000046.jpg</t>
+  </si>
+  <si>
+    <t>000047.jpg</t>
+  </si>
+  <si>
+    <t>000048.jpg</t>
+  </si>
+  <si>
+    <t>000049.jpg</t>
+  </si>
+  <si>
+    <t>000050.jpg</t>
+  </si>
+  <si>
+    <t>000051.jpg</t>
+  </si>
+  <si>
+    <t>000052.jpg</t>
+  </si>
+  <si>
+    <t>000053.jpg</t>
+  </si>
+  <si>
+    <t>000054.jpg</t>
+  </si>
+  <si>
+    <t>000055.jpg</t>
+  </si>
+  <si>
+    <t>000056.jpg</t>
+  </si>
+  <si>
+    <t>000057.jpg</t>
+  </si>
+  <si>
+    <t>000058.jpg</t>
+  </si>
+  <si>
+    <t>000059.jpg</t>
+  </si>
+  <si>
+    <t>000060.jpg</t>
+  </si>
+  <si>
+    <t>000061.jpg</t>
+  </si>
+  <si>
+    <t>000062.jpg</t>
+  </si>
+  <si>
+    <t>000063.jpg</t>
+  </si>
+  <si>
+    <t>000064.jpg</t>
+  </si>
+  <si>
+    <t>000065.jpg</t>
+  </si>
+  <si>
+    <t>000066.jpg</t>
+  </si>
+  <si>
+    <t>000067.jpg</t>
+  </si>
+  <si>
+    <t>000068.jpg</t>
+  </si>
+  <si>
+    <t>000069.jpg</t>
+  </si>
+  <si>
+    <t>000070.jpg</t>
+  </si>
+  <si>
+    <t>000071.jpg</t>
+  </si>
+  <si>
+    <t>000072.jpg</t>
+  </si>
+  <si>
+    <t>000073.jpg</t>
+  </si>
+  <si>
+    <t>000074.jpg</t>
+  </si>
+  <si>
+    <t>000075.jpg</t>
+  </si>
+  <si>
+    <t>000076.jpg</t>
+  </si>
+  <si>
+    <t>000077.jpg</t>
+  </si>
+  <si>
+    <t>000078.jpg</t>
+  </si>
+  <si>
+    <t>000079.jpg</t>
+  </si>
+  <si>
+    <t>000080.jpg</t>
+  </si>
+  <si>
+    <t>japan, India, Indian Prime Minister, japanese Prime Minister, kishida, Modi, Bilateral Relations, International Relations, Trade, Pact, Harmony</t>
   </si>
 </sst>
 </file>
@@ -500,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,7 +645,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,7 +653,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,7 +669,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +677,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,7 +685,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +693,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +701,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +709,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +717,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,7 +725,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,7 +733,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -633,7 +741,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +749,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -657,7 +765,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,7 +773,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +781,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +789,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -689,7 +797,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -697,7 +805,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -705,7 +813,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +821,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +829,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -729,7 +837,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +845,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +853,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +861,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +869,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +877,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +885,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -785,7 +893,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -793,7 +901,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -801,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -809,7 +917,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -817,7 +925,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -825,7 +933,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -833,7 +941,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,7 +949,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -849,7 +957,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -857,7 +965,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -865,10 +973,299 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding optimizations in js to accelerate the process
</commit_message>
<xml_diff>
--- a/Files_and_Tags.xlsx
+++ b/Files_and_Tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh16.Yadav\Desktop\github\DamnIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8001E5-0EEE-4FBA-AFE3-EA66FBE86561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66369507-246D-4515-8F6B-BB70430923B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>FileNames</t>
   </si>
@@ -160,115 +160,7 @@
     <t>000044.jpg</t>
   </si>
   <si>
-    <t>000045.jpg</t>
-  </si>
-  <si>
-    <t>000046.jpg</t>
-  </si>
-  <si>
-    <t>000047.jpg</t>
-  </si>
-  <si>
-    <t>000048.jpg</t>
-  </si>
-  <si>
-    <t>000049.jpg</t>
-  </si>
-  <si>
-    <t>000050.jpg</t>
-  </si>
-  <si>
-    <t>000051.jpg</t>
-  </si>
-  <si>
-    <t>000052.jpg</t>
-  </si>
-  <si>
-    <t>000053.jpg</t>
-  </si>
-  <si>
-    <t>000054.jpg</t>
-  </si>
-  <si>
-    <t>000055.jpg</t>
-  </si>
-  <si>
-    <t>000056.jpg</t>
-  </si>
-  <si>
-    <t>000057.jpg</t>
-  </si>
-  <si>
-    <t>000058.jpg</t>
-  </si>
-  <si>
-    <t>000059.jpg</t>
-  </si>
-  <si>
-    <t>000060.jpg</t>
-  </si>
-  <si>
-    <t>000061.jpg</t>
-  </si>
-  <si>
-    <t>000062.jpg</t>
-  </si>
-  <si>
-    <t>000063.jpg</t>
-  </si>
-  <si>
-    <t>000064.jpg</t>
-  </si>
-  <si>
-    <t>000065.jpg</t>
-  </si>
-  <si>
-    <t>000066.jpg</t>
-  </si>
-  <si>
-    <t>000067.jpg</t>
-  </si>
-  <si>
-    <t>000068.jpg</t>
-  </si>
-  <si>
-    <t>000069.jpg</t>
-  </si>
-  <si>
-    <t>000070.jpg</t>
-  </si>
-  <si>
-    <t>000071.jpg</t>
-  </si>
-  <si>
-    <t>000072.jpg</t>
-  </si>
-  <si>
-    <t>000073.jpg</t>
-  </si>
-  <si>
-    <t>000074.jpg</t>
-  </si>
-  <si>
-    <t>000075.jpg</t>
-  </si>
-  <si>
-    <t>000076.jpg</t>
-  </si>
-  <si>
-    <t>000077.jpg</t>
-  </si>
-  <si>
-    <t>000078.jpg</t>
-  </si>
-  <si>
-    <t>000079.jpg</t>
-  </si>
-  <si>
-    <t>000080.jpg</t>
-  </si>
-  <si>
-    <t>japan, India, Indian Prime Minister, japanese Prime Minister, kishida, Modi, Bilateral Relations, International Relations, Trade, Pact, Harmony</t>
+    <t>Anthony Albanese, Modi, Narendra Modi, Prime Minister, India, Australia, Bilateral Relation, International Relations, Trade Deal, Pact</t>
   </si>
 </sst>
 </file>
@@ -608,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +561,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +569,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -685,7 +577,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -693,7 +585,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -701,7 +593,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -709,7 +601,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +609,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +617,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +625,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -741,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -749,7 +641,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,7 +649,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -765,7 +657,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -773,7 +665,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -781,7 +673,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -789,7 +681,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -797,7 +689,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -805,7 +697,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -813,7 +705,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -821,7 +713,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -829,7 +721,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -837,7 +729,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -845,7 +737,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -853,7 +745,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -861,7 +753,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -869,7 +761,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -877,7 +769,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +777,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -893,7 +785,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -901,7 +793,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -909,7 +801,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -917,7 +809,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,7 +817,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -933,7 +825,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -941,7 +833,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -949,7 +841,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,7 +849,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -965,7 +857,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,299 +865,10 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B73" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>74</v>
-      </c>
-      <c r="B74" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>75</v>
-      </c>
-      <c r="B75" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>76</v>
-      </c>
-      <c r="B76" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>79</v>
-      </c>
-      <c r="B79" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B80" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>